<commit_message>
Added create file functionality
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Euan\Desktop\Projects\Text-File-Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542772D8-B3DA-4605-829B-9F4A9E131A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F446392A-7ECA-4A4A-908C-658AEB35FDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -371,7 +371,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>